<commit_message>
added dest well count to spreadsheet
</commit_message>
<xml_diff>
--- a/app/static/sampleTransferSpreadsheet.xlsx
+++ b/app/static/sampleTransferSpreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Source Plate Barcode</t>
   </si>
@@ -69,9 +69,6 @@
     <t>A5</t>
   </si>
   <si>
-    <t>A7</t>
-  </si>
-  <si>
     <t>A1</t>
   </si>
   <si>
@@ -81,10 +78,16 @@
     <t>A8</t>
   </si>
   <si>
-    <t>ssdest000000141jul17_C</t>
-  </si>
-  <si>
-    <t>ssdest000000141jul17_384_C</t>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>ssdest000000141jul17_E</t>
+  </si>
+  <si>
+    <t>ssdest000000141jul17_384_E</t>
+  </si>
+  <si>
+    <t>Dest Well Count</t>
   </si>
 </sst>
 </file>
@@ -154,8 +157,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -228,7 +245,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -257,6 +274,13 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -285,6 +309,13 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -614,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -628,9 +659,10 @@
     <col min="5" max="5" width="31" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" customWidth="1"/>
     <col min="7" max="7" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="35" customHeight="1">
+    <row r="1" spans="1:8" ht="35" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -652,8 +684,11 @@
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -668,10 +703,13 @@
         <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -688,8 +726,11 @@
       <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="H3">
+        <v>96</v>
+      </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -706,8 +747,11 @@
       <c r="G4" t="s">
         <v>11</v>
       </c>
+      <c r="H4">
+        <v>96</v>
+      </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -724,14 +768,17 @@
       <c r="G5" t="s">
         <v>14</v>
       </c>
+      <c r="H5">
+        <v>96</v>
+      </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -740,16 +787,19 @@
         <v>21</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="H6">
+        <v>384</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -759,6 +809,9 @@
       </c>
       <c r="G7" t="s">
         <v>12</v>
+      </c>
+      <c r="H7">
+        <v>384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>